<commit_message>
FDR RQ3 code update
Re-ran FDR corrections for RQ3 as these were incorrect.
</commit_message>
<xml_diff>
--- a/RQ3 combined findings.xlsx
+++ b/RQ3 combined findings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelbateman/Documents/GitHub/sex_differences_CSF_proteins_brain_structure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E4589E-39A1-B144-9163-65F1C9F244CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CC288B-0D34-464D-AC08-F7D86DB9B1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20000" windowHeight="17440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20000" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CCL5" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="17">
   <si>
     <t>Estimate</t>
   </si>
@@ -80,7 +80,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -225,6 +225,12 @@
       <i/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -570,7 +576,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -580,6 +586,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -937,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -992,8 +999,8 @@
       <c r="F2" s="1">
         <v>0.42415138646918599</v>
       </c>
-      <c r="G2" s="1">
-        <v>0.67175539736179701</v>
+      <c r="G2" s="5">
+        <v>0.86368551089373902</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1015,8 +1022,8 @@
       <c r="F3" s="1">
         <v>1.2904285402541</v>
       </c>
-      <c r="G3" s="1">
-        <v>0.19788575749373899</v>
+      <c r="G3" s="5">
+        <v>0.39259232958547502</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1038,8 +1045,8 @@
       <c r="F4" s="1">
         <v>0.78624688340160698</v>
       </c>
-      <c r="G4" s="1">
-        <v>0.43233529852756702</v>
+      <c r="G4" s="5">
+        <v>0.64850294779134998</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1061,8 +1068,8 @@
       <c r="F5" s="1">
         <v>-1.1278299352722001</v>
       </c>
-      <c r="G5" s="1">
-        <v>0.260281085962772</v>
+      <c r="G5" s="5">
+        <v>0.64850294779134998</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1084,8 +1091,8 @@
       <c r="F6" s="1">
         <v>0.90465999694105204</v>
       </c>
-      <c r="G6" s="1">
-        <v>0.36636190755395698</v>
+      <c r="G6" s="5">
+        <v>0.64850294779134998</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1107,8 +1114,8 @@
       <c r="F7" s="1">
         <v>2.1525727624758701</v>
       </c>
-      <c r="G7" s="1">
-        <v>3.2139055571925403E-2</v>
+      <c r="G7" s="5">
+        <v>0.28925150014732798</v>
       </c>
       <c r="H7" t="s">
         <v>13</v>
@@ -1133,7 +1140,7 @@
       <c r="F8" s="1">
         <v>0.13242818213375801</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="5">
         <v>0.89473323361632695</v>
       </c>
     </row>
@@ -1156,8 +1163,8 @@
       <c r="F9" s="1">
         <v>-0.13990905490531799</v>
       </c>
-      <c r="G9" s="1">
-        <v>0.888824801144393</v>
+      <c r="G9" s="5">
+        <v>0.89473323361632695</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -1179,8 +1186,8 @@
       <c r="F10" s="1">
         <v>-0.80239007120736405</v>
       </c>
-      <c r="G10" s="1">
-        <v>0.42295832055344701</v>
+      <c r="G10" s="5">
+        <v>0.64850294779134998</v>
       </c>
     </row>
   </sheetData>
@@ -1193,7 +1200,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:E10"/>
+      <selection activeCell="G2" sqref="G2:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1243,8 +1250,8 @@
       <c r="F2" s="1">
         <v>0.182791443641765</v>
       </c>
-      <c r="G2" s="1">
-        <v>0.85530755793842805</v>
+      <c r="G2" s="5">
+        <v>0.98860546879340805</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1266,8 +1273,8 @@
       <c r="F3" s="1">
         <v>1.99965998742369</v>
       </c>
-      <c r="G3" s="1">
-        <v>4.8095353572311601E-2</v>
+      <c r="G3" s="5">
+        <v>9.9487850918892298E-2</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
@@ -1292,8 +1299,8 @@
       <c r="F4" s="1">
         <v>0.67182327152355104</v>
       </c>
-      <c r="G4" s="1">
-        <v>0.50314419227044405</v>
+      <c r="G4" s="5">
+        <v>0.75471628840566696</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1315,8 +1322,8 @@
       <c r="F5" s="1">
         <v>-1.45016963343816</v>
       </c>
-      <c r="G5" s="1">
-        <v>0.149936234532661</v>
+      <c r="G5" s="5">
+        <v>0.39848108508763502</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1338,8 +1345,8 @@
       <c r="F6" s="1">
         <v>3.5819676790421799E-2</v>
       </c>
-      <c r="G6" s="1">
-        <v>0.97149288271064405</v>
+      <c r="G6" s="5">
+        <v>0.98860546879340805</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1361,8 +1368,8 @@
       <c r="F7" s="1">
         <v>1.3586884900798299</v>
       </c>
-      <c r="G7" s="1">
-        <v>0.17710270448339299</v>
+      <c r="G7" s="5">
+        <v>0.39848108508763502</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1384,8 +1391,8 @@
       <c r="F8" s="1">
         <v>-0.71557583031998795</v>
       </c>
-      <c r="G8" s="1">
-        <v>0.47581192610712397</v>
+      <c r="G8" s="5">
+        <v>0.75471628840566696</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1407,7 +1414,7 @@
       <c r="F9" s="1">
         <v>1.43151412446254E-2</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="5">
         <v>0.98860546879340805</v>
       </c>
     </row>
@@ -1430,8 +1437,8 @@
       <c r="F10" s="1">
         <v>-2.3067295539060799</v>
       </c>
-      <c r="G10" s="1">
-        <v>2.3014302430744201E-2</v>
+      <c r="G10" s="5">
+        <v>0.103564360938349</v>
       </c>
       <c r="H10" t="s">
         <v>13</v>
@@ -1444,10 +1451,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:E5"/>
+      <selection activeCell="G2" sqref="G2:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1455,7 +1462,7 @@
     <col min="8" max="8" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -1478,7 +1485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1497,11 +1504,11 @@
       <c r="F2" s="1">
         <v>-1.1747510897887099</v>
       </c>
-      <c r="G2" s="1">
-        <v>0.24108883964269401</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G2" s="5">
+        <v>0.36163325946404101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1520,11 +1527,11 @@
       <c r="F3" s="1">
         <v>0.22732408845881499</v>
       </c>
-      <c r="G3" s="1">
-        <v>0.82033763569224805</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G3" s="5">
+        <v>0.88083698415301703</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1543,11 +1550,11 @@
       <c r="F4" s="1">
         <v>-1.8141192967966999</v>
       </c>
-      <c r="G4" s="1">
-        <v>7.0725793753910499E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G4" s="5">
+        <v>0.16465098547288801</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1566,14 +1573,11 @@
       <c r="F5" s="1">
         <v>-2.1564801752391798</v>
       </c>
-      <c r="G5" s="1">
-        <v>3.18945362524048E-2</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G5" s="5">
+        <v>0.16465098547288801</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1592,11 +1596,11 @@
       <c r="F6" s="1">
         <v>-1.7984540600383001</v>
       </c>
-      <c r="G6" s="1">
-        <v>7.3178215765728E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G6" s="5">
+        <v>0.16465098547288801</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1615,11 +1619,11 @@
       <c r="F7" s="1">
         <v>-1.84936477863395</v>
       </c>
-      <c r="G7" s="1">
-        <v>6.5455218267895507E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G7" s="5">
+        <v>0.16465098547288801</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1638,11 +1642,11 @@
       <c r="F8" s="1">
         <v>-0.85824123568694299</v>
       </c>
-      <c r="G8" s="1">
-        <v>0.39149072433440901</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G8" s="5">
+        <v>0.50334521700138202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1661,11 +1665,11 @@
       <c r="F9" s="1">
         <v>1.5675833958696901</v>
       </c>
-      <c r="G9" s="1">
-        <v>0.118107787310508</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G9" s="5">
+        <v>0.21259401715891399</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1684,8 +1688,8 @@
       <c r="F10" s="1">
         <v>0.53482995052012205</v>
       </c>
-      <c r="G10" s="1">
-        <v>0.59319342546947995</v>
+      <c r="G10" s="5">
+        <v>0.667342603653165</v>
       </c>
     </row>
   </sheetData>
@@ -1695,10 +1699,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1706,7 +1710,7 @@
     <col min="8" max="8" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -1729,7 +1733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1748,14 +1752,11 @@
       <c r="F2" s="1">
         <v>-2.1636111516618701</v>
       </c>
-      <c r="G2" s="1">
-        <v>3.1336985404628898E-2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G2" s="5">
+        <v>0.28203286864166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1774,11 +1775,11 @@
       <c r="F3" s="1">
         <v>0.34281612441474801</v>
       </c>
-      <c r="G3" s="1">
-        <v>0.73199401564254996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G3" s="5">
+        <v>0.83910256252064996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1797,11 +1798,11 @@
       <c r="F4" s="1">
         <v>-1.60345660491088</v>
       </c>
-      <c r="G4" s="1">
-        <v>0.109957259455139</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G4" s="5">
+        <v>0.307102741296917</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1820,11 +1821,11 @@
       <c r="F5" s="1">
         <v>-1.26427144744373</v>
       </c>
-      <c r="G5" s="1">
-        <v>0.20718027426964999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G5" s="5">
+        <v>0.37292449368537001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1843,11 +1844,11 @@
       <c r="F6" s="1">
         <v>-0.88723332885478001</v>
       </c>
-      <c r="G6" s="1">
-        <v>0.37571203037554601</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G6" s="5">
+        <v>0.48305832476855898</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1866,11 +1867,11 @@
       <c r="F7" s="1">
         <v>-1.4932637674900899</v>
       </c>
-      <c r="G7" s="1">
-        <v>0.136490107243074</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G7" s="5">
+        <v>0.307102741296917</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1889,11 +1890,11 @@
       <c r="F8" s="1">
         <v>0.20322972906491801</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="5">
         <v>0.83910256252064996</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1912,11 +1913,11 @@
       <c r="F9" s="1">
         <v>0.96047895336333799</v>
       </c>
-      <c r="G9" s="1">
-        <v>0.33764288672492498</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G9" s="5">
+        <v>0.48305832476855898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1935,8 +1936,8 @@
       <c r="F10" s="1">
         <v>1.7931725642466101</v>
       </c>
-      <c r="G10" s="1">
-        <v>7.4028356122820493E-2</v>
+      <c r="G10" s="5">
+        <v>0.307102741296917</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RQ3 sex disaggregated findings
Updated code and excel file to show sex disaggregated findings for RQ3
</commit_message>
<xml_diff>
--- a/RQ3 combined findings.xlsx
+++ b/RQ3 combined findings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelbateman/Documents/GitHub/sex_differences_CSF_proteins_brain_structure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CC288B-0D34-464D-AC08-F7D86DB9B1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E80A43-34BA-AC46-B0AB-5C053D02417A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20000" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19160" windowHeight="17440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CCL5" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="21">
   <si>
     <t>Estimate</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Variables</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>heart_rate</t>
   </si>
   <si>
@@ -75,12 +72,63 @@
   <si>
     <t>97.5% CI</t>
   </si>
+  <si>
+    <t>Females Only:</t>
+  </si>
+  <si>
+    <t>Males Only:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>FDR-adj</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> p</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">FDR-adj </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>p</t>
+    </r>
+  </si>
+  <si>
+    <t>˚</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -231,6 +279,20 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -576,7 +638,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -587,6 +649,14 @@
     </xf>
     <xf numFmtId="11" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -942,19 +1012,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -965,10 +1035,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -976,11 +1046,14 @@
       <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1000,10 +1073,13 @@
         <v>0.42415138646918599</v>
       </c>
       <c r="G2" s="5">
+        <v>0.67175539736179701</v>
+      </c>
+      <c r="H2" s="5">
         <v>0.86368551089373902</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1023,10 +1099,13 @@
         <v>1.2904285402541</v>
       </c>
       <c r="G3" s="5">
+        <v>0.19788575749373899</v>
+      </c>
+      <c r="H3" s="5">
         <v>0.39259232958547502</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1046,10 +1125,13 @@
         <v>0.78624688340160698</v>
       </c>
       <c r="G4" s="5">
+        <v>0.43233529852756702</v>
+      </c>
+      <c r="H4" s="5">
         <v>0.64850294779134998</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1069,12 +1151,15 @@
         <v>-1.1278299352722001</v>
       </c>
       <c r="G5" s="5">
+        <v>0.260281085962772</v>
+      </c>
+      <c r="H5" s="5">
         <v>0.64850294779134998</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>4.4461587898826996E-3</v>
@@ -1092,10 +1177,13 @@
         <v>0.90465999694105204</v>
       </c>
       <c r="G6" s="5">
+        <v>0.36636190755395698</v>
+      </c>
+      <c r="H6" s="5">
         <v>0.64850294779134998</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1115,13 +1203,13 @@
         <v>2.1525727624758701</v>
       </c>
       <c r="G7" s="5">
+        <v>3.2139055571925403E-2</v>
+      </c>
+      <c r="H7" s="5">
         <v>0.28925150014732798</v>
       </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1143,8 +1231,11 @@
       <c r="G8" s="5">
         <v>0.89473323361632695</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H8" s="5">
+        <v>0.89473323361632695</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1164,10 +1255,13 @@
         <v>-0.13990905490531799</v>
       </c>
       <c r="G9" s="5">
+        <v>0.888824801144393</v>
+      </c>
+      <c r="H9" s="5">
         <v>0.89473323361632695</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1187,8 +1281,217 @@
         <v>-0.80239007120736405</v>
       </c>
       <c r="G10" s="5">
+        <v>0.42295832055344701</v>
+      </c>
+      <c r="H10" s="5">
         <v>0.64850294779134998</v>
       </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1197,15 +1500,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0244CAB-6277-F943-8B13-CF98041281F0}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G10"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -1219,16 +1523,19 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1251,6 +1558,9 @@
         <v>0.182791443641765</v>
       </c>
       <c r="G2" s="5">
+        <v>0.85530755793842805</v>
+      </c>
+      <c r="H2" s="5">
         <v>0.98860546879340805</v>
       </c>
     </row>
@@ -1274,10 +1584,10 @@
         <v>1.99965998742369</v>
       </c>
       <c r="G3" s="5">
+        <v>4.8095353572311601E-2</v>
+      </c>
+      <c r="H3" s="5">
         <v>9.9487850918892298E-2</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1300,6 +1610,9 @@
         <v>0.67182327152355104</v>
       </c>
       <c r="G4" s="5">
+        <v>0.50314419227044405</v>
+      </c>
+      <c r="H4" s="5">
         <v>0.75471628840566696</v>
       </c>
     </row>
@@ -1323,12 +1636,15 @@
         <v>-1.45016963343816</v>
       </c>
       <c r="G5" s="5">
+        <v>0.149936234532661</v>
+      </c>
+      <c r="H5" s="5">
         <v>0.39848108508763502</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>1.8405993971989099E-4</v>
@@ -1346,6 +1662,9 @@
         <v>3.5819676790421799E-2</v>
       </c>
       <c r="G6" s="5">
+        <v>0.97149288271064405</v>
+      </c>
+      <c r="H6" s="5">
         <v>0.98860546879340805</v>
       </c>
     </row>
@@ -1369,6 +1688,9 @@
         <v>1.3586884900798299</v>
       </c>
       <c r="G7" s="5">
+        <v>0.17710270448339299</v>
+      </c>
+      <c r="H7" s="5">
         <v>0.39848108508763502</v>
       </c>
     </row>
@@ -1392,6 +1714,9 @@
         <v>-0.71557583031998795</v>
       </c>
       <c r="G8" s="5">
+        <v>0.47581192610712397</v>
+      </c>
+      <c r="H8" s="5">
         <v>0.75471628840566696</v>
       </c>
     </row>
@@ -1417,6 +1742,9 @@
       <c r="G9" s="5">
         <v>0.98860546879340805</v>
       </c>
+      <c r="H9" s="5">
+        <v>0.98860546879340805</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -1438,10 +1766,557 @@
         <v>-2.3067295539060799</v>
       </c>
       <c r="G10" s="5">
+        <v>2.3014302430744201E-2</v>
+      </c>
+      <c r="H10" s="5">
         <v>0.103564360938349</v>
       </c>
-      <c r="H10" t="s">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="5">
+        <v>3.8403058859326197E-2</v>
+      </c>
+      <c r="C14" s="5">
+        <v>2.8007474271691198E-2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-1.829511E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>9.5101229999999995E-2</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1.3711717981704099</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.178365196610413</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0.60286004606229704</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="5">
+        <v>9.8048115343507297E-2</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.144557706083738</v>
+      </c>
+      <c r="D15" s="1">
+        <v>-0.19459366</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.39068988999999998</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.67826280590472998</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0.50171478254530399</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0.672382927674675</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="5">
+        <v>8.7914138149519806E-3</v>
+      </c>
+      <c r="C16" s="5">
+        <v>2.5548146010600101E-2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>-4.2928099999999997E-2</v>
+      </c>
+      <c r="E16" s="1">
+        <v>6.0510929999999997E-2</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.344111616212948</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0.73265936098083295</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0.753078627461928</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="5">
+        <v>-0.22435408955890501</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.19954995927094099</v>
+      </c>
+      <c r="D17" s="1">
+        <v>-0.62832186000000001</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.17961368</v>
+      </c>
+      <c r="F17" s="5">
+        <v>-1.1243003525462301</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.26793779824990999</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0.60286004606229704</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="B18" s="5">
+        <v>-6.7851689223779304E-3</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1.0523764435143201E-2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>-2.808942E-2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1.451908E-2</v>
+      </c>
+      <c r="F18" s="5">
+        <v>-0.644747320618415</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.52296449930252498</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0.672382927674675</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1.2821610180032099E-2</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1.1083764693858701E-2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>-9.6162980000000006E-3</v>
+      </c>
+      <c r="E19" s="1">
+        <v>3.5259520000000003E-2</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1.15679198667365</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.25457785213971701</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0.60286004606229704</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="5">
+        <v>-2.2898393451272802E-3</v>
+      </c>
+      <c r="C20" s="5">
+        <v>7.2264929605149499E-3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>-1.6919110000000001E-2</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1.233943E-2</v>
+      </c>
+      <c r="F20" s="5">
+        <v>-0.31686730446411598</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0.753078627461928</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0.753078627461928</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1.02760208302252E-2</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1.15762299161135E-2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>-1.315883E-2</v>
+      </c>
+      <c r="E21" s="1">
+        <v>3.3710869999999997E-2</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.88768285570430505</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0.38029565690838801</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0.672382927674675</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="5">
+        <v>-1.1344191414002201E-2</v>
+      </c>
+      <c r="C22" s="5">
+        <v>7.10514853904549E-3</v>
+      </c>
+      <c r="D22" s="1">
+        <v>-2.5740590000000001E-2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>3.0522069999999999E-3</v>
+      </c>
+      <c r="F22" s="5">
+        <v>-1.59661565858357</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0.118858265396673</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0.60286004606229704</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="5">
+        <v>-1.46740450053231E-2</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1.7311976594541999E-2</v>
+      </c>
+      <c r="D26" s="5">
+        <v>-4.9258690000000001E-2</v>
+      </c>
+      <c r="E26" s="5">
+        <v>1.9910600000000001E-2</v>
+      </c>
+      <c r="F26" s="5">
+        <v>-0.84762389350442102</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0.39980628564854698</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0.58604428053588198</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="5">
+        <v>0.27523142034155901</v>
+      </c>
+      <c r="C27" s="5">
+        <v>9.6823977953718998E-2</v>
+      </c>
+      <c r="D27" s="5">
+        <v>8.1803288000000002E-2</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0.46865954999999998</v>
+      </c>
+      <c r="F27" s="5">
+        <v>2.8425956685348899</v>
+      </c>
+      <c r="G27" s="5">
+        <v>5.9981093166464102E-3</v>
+      </c>
+      <c r="H27" s="5">
+        <v>5.3982983849817701E-2</v>
+      </c>
+      <c r="I27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="5">
+        <v>1.2175601220615499E-2</v>
+      </c>
+      <c r="C28" s="5">
+        <v>1.70801734942858E-2</v>
+      </c>
+      <c r="D28" s="5">
+        <v>-2.1945969999999999E-2</v>
+      </c>
+      <c r="E28" s="5">
+        <v>4.6297169999999999E-2</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0.71284997337344902</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0.47852969643176502</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0.58604428053588198</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="5">
+        <v>-0.15227523982900601</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0.124635978755434</v>
+      </c>
+      <c r="D29" s="5">
+        <v>-0.40126423</v>
+      </c>
+      <c r="E29" s="5">
+        <v>9.6713750000000001E-2</v>
+      </c>
+      <c r="F29" s="5">
+        <v>-1.22175989108095</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0.226279588916554</v>
+      </c>
+      <c r="H29" s="5">
+        <v>0.58604428053588198</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="5">
+        <v>3.9112890936827804E-3</v>
+      </c>
+      <c r="C30" s="5">
+        <v>6.0595712543511596E-3</v>
+      </c>
+      <c r="D30" s="5">
+        <v>-8.1940959999999997E-3</v>
+      </c>
+      <c r="E30" s="5">
+        <v>1.601667E-2</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0.64547291045950195</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0.52092824936522797</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0.58604428053588198</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="5">
+        <v>5.46300444822657E-3</v>
+      </c>
+      <c r="C31" s="5">
+        <v>6.8843675853726503E-3</v>
+      </c>
+      <c r="D31" s="5">
+        <v>-8.2901009999999994E-3</v>
+      </c>
+      <c r="E31" s="5">
+        <v>1.9216110000000002E-2</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0.79353758794546603</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0.430396979671341</v>
+      </c>
+      <c r="H31" s="5">
+        <v>0.58604428053588198</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="5">
+        <v>-2.4205705407434699E-3</v>
+      </c>
+      <c r="C32" s="5">
+        <v>3.5301511109626701E-3</v>
+      </c>
+      <c r="D32" s="5">
+        <v>-9.4728580000000007E-3</v>
+      </c>
+      <c r="E32" s="5">
+        <v>4.6317169999999996E-3</v>
+      </c>
+      <c r="F32" s="5">
+        <v>-0.68568468166321195</v>
+      </c>
+      <c r="G32" s="5">
+        <v>0.49538834297712198</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0.58604428053588198</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="5">
+        <v>-3.85800046848337E-3</v>
+      </c>
+      <c r="C33" s="5">
+        <v>7.1564475398936504E-3</v>
+      </c>
+      <c r="D33" s="5">
+        <v>-1.8159020000000001E-2</v>
+      </c>
+      <c r="E33" s="5">
+        <v>1.0443020000000001E-2</v>
+      </c>
+      <c r="F33" s="5">
+        <v>-0.53909435470279599</v>
+      </c>
+      <c r="G33" s="5">
+        <v>0.59172184316946297</v>
+      </c>
+      <c r="H33" s="5">
+        <v>0.59172184316946297</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="5">
+        <v>-1.08099694424191E-2</v>
+      </c>
+      <c r="C34" s="5">
+        <v>6.8411539260034102E-3</v>
+      </c>
+      <c r="D34" s="5">
+        <v>-2.4476749999999999E-2</v>
+      </c>
+      <c r="E34" s="5">
+        <v>2.8568069999999998E-3</v>
+      </c>
+      <c r="F34" s="5">
+        <v>-1.58013831574965</v>
+      </c>
+      <c r="G34" s="5">
+        <v>0.119005266277724</v>
+      </c>
+      <c r="H34" s="5">
+        <v>0.53552369824975699</v>
       </c>
     </row>
   </sheetData>
@@ -1451,18 +2326,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G10"/>
+    <sheetView topLeftCell="A17" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -1473,10 +2348,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -1484,8 +2359,11 @@
       <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1505,10 +2383,13 @@
         <v>-1.1747510897887099</v>
       </c>
       <c r="G2" s="5">
+        <v>0.24108883964269401</v>
+      </c>
+      <c r="H2" s="5">
         <v>0.36163325946404101</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1528,10 +2409,13 @@
         <v>0.22732408845881499</v>
       </c>
       <c r="G3" s="5">
+        <v>0.82033763569224805</v>
+      </c>
+      <c r="H3" s="5">
         <v>0.88083698415301703</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1551,10 +2435,13 @@
         <v>-1.8141192967966999</v>
       </c>
       <c r="G4" s="5">
+        <v>7.0725793753910499E-2</v>
+      </c>
+      <c r="H4" s="5">
         <v>0.16465098547288801</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1574,12 +2461,15 @@
         <v>-2.1564801752391798</v>
       </c>
       <c r="G5" s="5">
+        <v>3.18945362524048E-2</v>
+      </c>
+      <c r="H5" s="5">
         <v>0.16465098547288801</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>-1.0671941246508601E-2</v>
@@ -1597,10 +2487,13 @@
         <v>-1.7984540600383001</v>
       </c>
       <c r="G6" s="5">
+        <v>7.3178215765728E-2</v>
+      </c>
+      <c r="H6" s="5">
         <v>0.16465098547288801</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1620,10 +2513,13 @@
         <v>-1.84936477863395</v>
       </c>
       <c r="G7" s="5">
+        <v>6.5455218267895507E-2</v>
+      </c>
+      <c r="H7" s="5">
         <v>0.16465098547288801</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1643,10 +2539,13 @@
         <v>-0.85824123568694299</v>
       </c>
       <c r="G8" s="5">
+        <v>0.39149072433440901</v>
+      </c>
+      <c r="H8" s="5">
         <v>0.50334521700138202</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1666,10 +2565,13 @@
         <v>1.5675833958696901</v>
       </c>
       <c r="G9" s="5">
+        <v>0.118107787310508</v>
+      </c>
+      <c r="H9" s="5">
         <v>0.21259401715891399</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1689,7 +2591,554 @@
         <v>0.53482995052012205</v>
       </c>
       <c r="G10" s="5">
+        <v>0.59319342546947995</v>
+      </c>
+      <c r="H10" s="5">
         <v>0.667342603653165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="5">
+        <v>5.5901802243496501E-2</v>
+      </c>
+      <c r="C14" s="5">
+        <v>3.4053352909623101E-2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-1.159084E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.12339443999999999</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1.6415946585893799</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.103556325364002</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0.56061257483864002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="5">
+        <v>-2.28578746748242E-2</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.15718651542956999</v>
+      </c>
+      <c r="D15" s="1">
+        <v>-0.33439644000000002</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.28868069000000002</v>
+      </c>
+      <c r="F15" s="5">
+        <v>-0.145418801430623</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0.88464879196771995</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0.88464879196771995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="5">
+        <v>-3.3124906532570199E-2</v>
+      </c>
+      <c r="C16" s="5">
+        <v>2.45581374917762E-2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>-8.1798339999999997E-2</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1.554852E-2</v>
+      </c>
+      <c r="F16" s="5">
+        <v>-1.34883626837185</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0.180185182202593</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0.56061257483864002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="5">
+        <v>-0.15631586135072001</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.21428547823160199</v>
+      </c>
+      <c r="D17" s="1">
+        <v>-0.58102271000000005</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.26839099</v>
+      </c>
+      <c r="F17" s="5">
+        <v>-0.72947482321584201</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.46727594439889902</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0.70091391659834801</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="5">
+        <v>-4.2977281733790904E-3</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1.12257615605636E-2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>-2.6546819999999999E-2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1.7951370000000001E-2</v>
+      </c>
+      <c r="F18" s="5">
+        <v>-0.38284513261684899</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.70258015721775802</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0.79040267686997701</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="5">
+        <v>-1.15080030166955E-2</v>
+      </c>
+      <c r="C19" s="5">
+        <v>9.7273050362463604E-3</v>
+      </c>
+      <c r="D19" s="1">
+        <v>-3.0787209999999999E-2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>7.7711990000000003E-3</v>
+      </c>
+      <c r="F19" s="5">
+        <v>-1.18306180116834</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.23935863854473</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0.56061257483864002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="5">
+        <v>-6.5962257975806298E-3</v>
+      </c>
+      <c r="C20" s="5">
+        <v>5.69339103826242E-3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>-1.7880340000000002E-2</v>
+      </c>
+      <c r="E20" s="1">
+        <v>4.6878900000000001E-3</v>
+      </c>
+      <c r="F20" s="5">
+        <v>-1.1585759265876401</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0.24916114437272899</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0.56061257483864002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="5">
+        <v>8.4341987006811402E-3</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1.10104168913783E-2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>-1.338809E-2</v>
+      </c>
+      <c r="E21" s="1">
+        <v>3.025649E-2</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.76601992312257905</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0.44532013989089098</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0.70091391659834801</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="5">
+        <v>3.8978544145989E-3</v>
+      </c>
+      <c r="C22" s="5">
+        <v>8.6550940871676797E-3</v>
+      </c>
+      <c r="D22" s="1">
+        <v>-1.325804E-2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2.105375E-2</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0.45035378880259502</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0.65335811040796998</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0.79040267686997701</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="5">
+        <v>-6.6115768733098698E-2</v>
+      </c>
+      <c r="C26" s="5">
+        <v>2.5148671107481702E-2</v>
+      </c>
+      <c r="D26" s="5">
+        <v>-0.11576606</v>
+      </c>
+      <c r="E26" s="5">
+        <v>-1.6465480000000001E-2</v>
+      </c>
+      <c r="F26" s="5">
+        <v>-2.6289965163777298</v>
+      </c>
+      <c r="G26" s="5">
+        <v>9.3629692319544405E-3</v>
+      </c>
+      <c r="H26" s="5">
+        <v>8.4266723087590006E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="5">
+        <v>3.0983534284012099E-2</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0.11456910969949</v>
+      </c>
+      <c r="D27" s="5">
+        <v>-0.19520693</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0.25717400000000001</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0.27043532384322999</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0.78715929686626795</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0.88555420897455095</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="5">
+        <v>-2.34857847921074E-2</v>
+      </c>
+      <c r="C28" s="5">
+        <v>2.10208131770926E-2</v>
+      </c>
+      <c r="D28" s="5">
+        <v>-6.4986569999999994E-2</v>
+      </c>
+      <c r="E28" s="5">
+        <v>1.8015E-2</v>
+      </c>
+      <c r="F28" s="5">
+        <v>-1.1172633805480501</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0.265486518097302</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0.39822977714595298</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="5">
+        <v>-0.30558317590038397</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0.150938520876159</v>
+      </c>
+      <c r="D29" s="5">
+        <v>-0.60357669999999997</v>
+      </c>
+      <c r="E29" s="5">
+        <v>-7.5896380000000001E-3</v>
+      </c>
+      <c r="F29" s="5">
+        <v>-2.02455393180318</v>
+      </c>
+      <c r="G29" s="5">
+        <v>4.4506410794346501E-2</v>
+      </c>
+      <c r="H29" s="5">
+        <v>0.142108611957286</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="5">
+        <v>-1.4258118316252601E-2</v>
+      </c>
+      <c r="C30" s="5">
+        <v>7.1371625211148204E-3</v>
+      </c>
+      <c r="D30" s="5">
+        <v>-2.8348809999999999E-2</v>
+      </c>
+      <c r="E30" s="5">
+        <v>-1.6742560000000001E-4</v>
+      </c>
+      <c r="F30" s="5">
+        <v>-1.9977292480129101</v>
+      </c>
+      <c r="G30" s="5">
+        <v>4.7369537319095503E-2</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0.142108611957286</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="5">
+        <v>-1.14925850438216E-2</v>
+      </c>
+      <c r="C31" s="5">
+        <v>8.4229095075988494E-3</v>
+      </c>
+      <c r="D31" s="5">
+        <v>-2.8121690000000001E-2</v>
+      </c>
+      <c r="E31" s="5">
+        <v>5.1365209999999998E-3</v>
+      </c>
+      <c r="F31" s="5">
+        <v>-1.3644436086430001</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0.174263795838587</v>
+      </c>
+      <c r="H31" s="5">
+        <v>0.35071503371006002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="5">
+        <v>-5.9867798111030795E-4</v>
+      </c>
+      <c r="C32" s="5">
+        <v>4.1672640863976802E-3</v>
+      </c>
+      <c r="D32" s="5">
+        <v>-8.8259859999999992E-3</v>
+      </c>
+      <c r="E32" s="5">
+        <v>7.62863E-3</v>
+      </c>
+      <c r="F32" s="5">
+        <v>-0.143662117086471</v>
+      </c>
+      <c r="G32" s="5">
+        <v>0.88594049342070702</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0.88594049342070702</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="5">
+        <v>1.27881687176301E-2</v>
+      </c>
+      <c r="C33" s="5">
+        <v>9.8246306131965708E-3</v>
+      </c>
+      <c r="D33" s="5">
+        <v>-6.609167E-3</v>
+      </c>
+      <c r="E33" s="5">
+        <v>3.2185499999999999E-2</v>
+      </c>
+      <c r="F33" s="5">
+        <v>1.3016437178261899</v>
+      </c>
+      <c r="G33" s="5">
+        <v>0.19484168539447799</v>
+      </c>
+      <c r="H33" s="5">
+        <v>0.35071503371006002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="5">
+        <v>2.3592845610183699E-3</v>
+      </c>
+      <c r="C34" s="5">
+        <v>7.3584317369427997E-3</v>
+      </c>
+      <c r="D34" s="5">
+        <v>-1.216889E-2</v>
+      </c>
+      <c r="E34" s="5">
+        <v>1.688746E-2</v>
+      </c>
+      <c r="F34" s="5">
+        <v>0.32062328568921</v>
+      </c>
+      <c r="G34" s="5">
+        <v>0.74889914820379899</v>
+      </c>
+      <c r="H34" s="5">
+        <v>0.88555420897455095</v>
       </c>
     </row>
   </sheetData>
@@ -1699,18 +3148,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -1721,10 +3170,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -1732,8 +3181,11 @@
       <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1753,10 +3205,13 @@
         <v>-2.1636111516618701</v>
       </c>
       <c r="G2" s="5">
+        <v>3.1336985404628898E-2</v>
+      </c>
+      <c r="H2" s="5">
         <v>0.28203286864166</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1776,10 +3231,13 @@
         <v>0.34281612441474801</v>
       </c>
       <c r="G3" s="5">
+        <v>0.73199401564254996</v>
+      </c>
+      <c r="H3" s="5">
         <v>0.83910256252064996</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1799,10 +3257,13 @@
         <v>-1.60345660491088</v>
       </c>
       <c r="G4" s="5">
+        <v>0.109957259455139</v>
+      </c>
+      <c r="H4" s="5">
         <v>0.307102741296917</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1822,12 +3283,15 @@
         <v>-1.26427144744373</v>
       </c>
       <c r="G5" s="5">
+        <v>0.20718027426964999</v>
+      </c>
+      <c r="H5" s="5">
         <v>0.37292449368537001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>-5.1874226160833203E-3</v>
@@ -1845,10 +3309,13 @@
         <v>-0.88723332885478001</v>
       </c>
       <c r="G6" s="5">
+        <v>0.37571203037554601</v>
+      </c>
+      <c r="H6" s="5">
         <v>0.48305832476855898</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1868,10 +3335,13 @@
         <v>-1.4932637674900899</v>
       </c>
       <c r="G7" s="5">
+        <v>0.136490107243074</v>
+      </c>
+      <c r="H7" s="5">
         <v>0.307102741296917</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1893,8 +3363,11 @@
       <c r="G8" s="5">
         <v>0.83910256252064996</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="5">
+        <v>0.83910256252064996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1914,10 +3387,13 @@
         <v>0.96047895336333799</v>
       </c>
       <c r="G9" s="5">
+        <v>0.33764288672492498</v>
+      </c>
+      <c r="H9" s="5">
         <v>0.48305832476855898</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1937,7 +3413,554 @@
         <v>1.7931725642466101</v>
       </c>
       <c r="G10" s="5">
+        <v>7.4028356122820493E-2</v>
+      </c>
+      <c r="H10" s="5">
         <v>0.307102741296917</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="5">
+        <v>-5.4560950628946897E-3</v>
+      </c>
+      <c r="C14" s="5">
+        <v>3.42941675873275E-2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-7.3426019999999995E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>6.2513830000000006E-2</v>
+      </c>
+      <c r="F14" s="5">
+        <v>-0.159096879928669</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.87388696274376398</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0.87388696274376398</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.15098510542975099</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.155740142006358</v>
+      </c>
+      <c r="D15" s="1">
+        <v>-0.15768679299999999</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.45965699999999998</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.96946813765963002</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0.33445797690312001</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0.84635786462936002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="5">
+        <v>-3.9607619799586401E-2</v>
+      </c>
+      <c r="C16" s="5">
+        <v>2.43437161507968E-2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>-8.7856074000000006E-2</v>
+      </c>
+      <c r="E16" s="1">
+        <v>8.640834E-3</v>
+      </c>
+      <c r="F16" s="5">
+        <v>-1.6270161693571199</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0.10662116508256</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0.84635786462936002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="5">
+        <v>-0.162200058590215</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.21316079845329899</v>
+      </c>
+      <c r="D17" s="1">
+        <v>-0.58467783100000004</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.26027771</v>
+      </c>
+      <c r="F17" s="5">
+        <v>-0.76092818082472502</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.44834298425821401</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0.84635786462936002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="5">
+        <v>-5.6649471458600697E-3</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1.11635605935613E-2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>-2.7790761000000001E-2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1.6460869999999999E-2</v>
+      </c>
+      <c r="F18" s="5">
+        <v>-0.507449849748422</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.61286442965794297</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0.84635786462936002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="5">
+        <v>-5.7642342713009401E-3</v>
+      </c>
+      <c r="C19" s="5">
+        <v>9.7246010599016299E-3</v>
+      </c>
+      <c r="D19" s="1">
+        <v>-2.5038076999999999E-2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1.350961E-2</v>
+      </c>
+      <c r="F19" s="5">
+        <v>-0.592747634149143</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.55457782841576198</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0.84635786462936002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1.7821423617241101E-3</v>
+      </c>
+      <c r="C20" s="5">
+        <v>5.6969371107627497E-3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>-9.5090020000000008E-3</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1.307329E-2</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0.31282465069822402</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0.75501162068937899</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0.84938807327555099</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="5">
+        <v>7.8314125202552307E-3</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1.0958777728682499E-2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>-1.3888529E-2</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2.9551350000000001E-2</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.71462463370873996</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0.47636872825696103</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0.84635786462936002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="5">
+        <v>3.8040663522103399E-3</v>
+      </c>
+      <c r="C22" s="5">
+        <v>8.5770278920045805E-3</v>
+      </c>
+      <c r="D22" s="1">
+        <v>-1.3197090999999999E-2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2.0805219999999999E-2</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0.44351801114654799</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0.65827833915616896</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0.84635786462936002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="5">
+        <v>-6.09530065770406E-2</v>
+      </c>
+      <c r="C26" s="5">
+        <v>2.4446551938260501E-2</v>
+      </c>
+      <c r="D26" s="5">
+        <v>-0.109217124</v>
+      </c>
+      <c r="E26" s="5">
+        <v>-1.268889E-2</v>
+      </c>
+      <c r="F26" s="5">
+        <v>-2.4933171242708099</v>
+      </c>
+      <c r="G26" s="5">
+        <v>1.3629390786314E-2</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0.122664517076826</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="5">
+        <v>-4.7641204449744401E-2</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0.11111092307353999</v>
+      </c>
+      <c r="D27" s="5">
+        <v>-0.26700426999999999</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0.17172186</v>
+      </c>
+      <c r="F27" s="5">
+        <v>-0.42877156567417402</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0.66864203689585</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0.75222229150783104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="5">
+        <v>-1.2711708463153599E-2</v>
+      </c>
+      <c r="C28" s="5">
+        <v>2.0445493571691498E-2</v>
+      </c>
+      <c r="D28" s="5">
+        <v>-5.3076653000000001E-2</v>
+      </c>
+      <c r="E28" s="5">
+        <v>2.7653239999999999E-2</v>
+      </c>
+      <c r="F28" s="5">
+        <v>-0.62173644370972803</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0.53496302042111799</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0.75222229150783104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="5">
+        <v>-0.119563243198955</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0.14792808630937099</v>
+      </c>
+      <c r="D29" s="5">
+        <v>-0.41161336799999998</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0.17248688000000001</v>
+      </c>
+      <c r="F29" s="5">
+        <v>-0.80825248390562099</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0.42009511137010302</v>
+      </c>
+      <c r="H29" s="5">
+        <v>0.75222229150783104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="5">
+        <v>-5.9394303787938703E-3</v>
+      </c>
+      <c r="C30" s="5">
+        <v>6.9911798982853898E-3</v>
+      </c>
+      <c r="D30" s="5">
+        <v>-1.9741913999999999E-2</v>
+      </c>
+      <c r="E30" s="5">
+        <v>7.8630530000000001E-3</v>
+      </c>
+      <c r="F30" s="5">
+        <v>-0.84956051270409005</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0.396785732927322</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0.75222229150783104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="5">
+        <v>-1.17030208312872E-2</v>
+      </c>
+      <c r="C31" s="5">
+        <v>8.1667389827014096E-3</v>
+      </c>
+      <c r="D31" s="5">
+        <v>-2.7826376E-2</v>
+      </c>
+      <c r="E31" s="5">
+        <v>4.4203350000000001E-3</v>
+      </c>
+      <c r="F31" s="5">
+        <v>-1.4330102695918501</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0.15372428843317201</v>
+      </c>
+      <c r="H31" s="5">
+        <v>0.46117286529951701</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="9">
+        <v>-6.5053255363152094E-5</v>
+      </c>
+      <c r="C32" s="5">
+        <v>4.0430636824946697E-3</v>
+      </c>
+      <c r="D32" s="5">
+        <v>-8.0471559999999998E-3</v>
+      </c>
+      <c r="E32" s="5">
+        <v>7.9170500000000001E-3</v>
+      </c>
+      <c r="F32" s="5">
+        <v>-1.60900892174453E-2</v>
+      </c>
+      <c r="G32" s="5">
+        <v>0.98718172675546501</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0.98718172675546501</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="5">
+        <v>4.4613414519017102E-3</v>
+      </c>
+      <c r="C33" s="5">
+        <v>9.5777920920158792E-3</v>
+      </c>
+      <c r="D33" s="5">
+        <v>-1.4448647E-2</v>
+      </c>
+      <c r="E33" s="5">
+        <v>2.3371329999999999E-2</v>
+      </c>
+      <c r="F33" s="5">
+        <v>0.46580061553233298</v>
+      </c>
+      <c r="G33" s="5">
+        <v>0.64196880449980098</v>
+      </c>
+      <c r="H33" s="5">
+        <v>0.75222229150783104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="5">
+        <v>1.3691189985754301E-2</v>
+      </c>
+      <c r="C34" s="5">
+        <v>7.0897413053843897E-3</v>
+      </c>
+      <c r="D34" s="5">
+        <v>-3.064958E-4</v>
+      </c>
+      <c r="E34" s="5">
+        <v>2.7688879999999999E-2</v>
+      </c>
+      <c r="F34" s="5">
+        <v>1.93112687699287</v>
+      </c>
+      <c r="G34" s="5">
+        <v>5.51710906871688E-2</v>
+      </c>
+      <c r="H34" s="5">
+        <v>0.24826990809225999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>